<commit_message>
EDD files for DBTL0.1
</commit_message>
<xml_diff>
--- a/data/flaviolin/DBTL0.1/experiment_description.xlsx
+++ b/data/flaviolin/DBTL0.1/experiment_description.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,21 +50,22 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -483,7 +484,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C0_WA1_biomek-R1</t>
+          <t>C0.1_WA1_biomek-R1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -509,7 +510,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -520,7 +521,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C0_WB1_biomek-R2</t>
+          <t>C0.1_WB1_biomek-R2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -546,7 +547,7 @@
         <v>30</v>
       </c>
       <c r="H3" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -557,7 +558,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C0_WC1_biomek-R3</t>
+          <t>C0.1_WC1_biomek-R3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -583,7 +584,7 @@
         <v>30</v>
       </c>
       <c r="H4" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -594,7 +595,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C0_WD1_biomek-R4</t>
+          <t>C0.1_WD1_biomek-R4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -620,7 +621,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -631,7 +632,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C0_WE1_biomek-R5</t>
+          <t>C0.1_WE1_biomek-R5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -657,7 +658,7 @@
         <v>30</v>
       </c>
       <c r="H6" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -668,7 +669,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C0_WF1_biomek-R6</t>
+          <t>C0.1_WF1_biomek-R6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -694,7 +695,7 @@
         <v>30</v>
       </c>
       <c r="H7" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -705,7 +706,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C0_WA2_biomek-R7</t>
+          <t>C0.1_WA2_biomek-R7</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -731,7 +732,7 @@
         <v>30</v>
       </c>
       <c r="H8" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -742,7 +743,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>C0_WB2_biomek-R8</t>
+          <t>C0.1_WB2_biomek-R8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -768,7 +769,7 @@
         <v>30</v>
       </c>
       <c r="H9" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -779,7 +780,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C0_WC2_biomek-R9</t>
+          <t>C0.1_WC2_biomek-R9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -805,7 +806,7 @@
         <v>30</v>
       </c>
       <c r="H10" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -816,7 +817,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C0_WD2_biomek-R10</t>
+          <t>C0.1_WD2_biomek-R10</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -842,7 +843,7 @@
         <v>30</v>
       </c>
       <c r="H11" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -853,7 +854,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C0_WE2_biomek-R11</t>
+          <t>C0.1_WE2_biomek-R11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -879,7 +880,7 @@
         <v>30</v>
       </c>
       <c r="H12" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -890,7 +891,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C0_WF2_biomek-R12</t>
+          <t>C0.1_WF2_biomek-R12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -916,7 +917,7 @@
         <v>30</v>
       </c>
       <c r="H13" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -927,7 +928,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C0_WA3_biomek-R13</t>
+          <t>C0.1_WA3_biomek-R13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -953,7 +954,7 @@
         <v>30</v>
       </c>
       <c r="H14" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -964,7 +965,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C0_WB3_biomek-R14</t>
+          <t>C0.1_WB3_biomek-R14</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -990,7 +991,7 @@
         <v>30</v>
       </c>
       <c r="H15" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1001,7 +1002,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C0_WC3_biomek-R15</t>
+          <t>C0.1_WC3_biomek-R15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1027,7 +1028,7 @@
         <v>30</v>
       </c>
       <c r="H16" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1038,7 +1039,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C0_WD3_biomek-R16</t>
+          <t>C0.1_WD3_biomek-R16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1064,7 +1065,7 @@
         <v>30</v>
       </c>
       <c r="H17" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1075,7 +1076,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C0_WE3_biomek-R17</t>
+          <t>C0.1_WE3_biomek-R17</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1101,7 +1102,7 @@
         <v>30</v>
       </c>
       <c r="H18" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1112,7 +1113,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C0_WF3_biomek-R18</t>
+          <t>C0.1_WF3_biomek-R18</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1138,7 +1139,7 @@
         <v>30</v>
       </c>
       <c r="H19" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1149,7 +1150,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C0_WA4_biomek-R19</t>
+          <t>C0.1_WA4_biomek-R19</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1175,7 +1176,7 @@
         <v>30</v>
       </c>
       <c r="H20" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1186,7 +1187,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C0_WB4_biomek-R20</t>
+          <t>C0.1_WB4_biomek-R20</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1212,7 +1213,7 @@
         <v>30</v>
       </c>
       <c r="H21" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1223,7 +1224,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C0_WC4_biomek-R21</t>
+          <t>C0.1_WC4_biomek-R21</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1249,7 +1250,7 @@
         <v>30</v>
       </c>
       <c r="H22" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1260,7 +1261,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C0_WD4_biomek-R22</t>
+          <t>C0.1_WD4_biomek-R22</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1286,7 +1287,7 @@
         <v>30</v>
       </c>
       <c r="H23" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1297,7 +1298,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>C0_WE4_biomek-R23</t>
+          <t>C0.1_WE4_biomek-R23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1323,7 +1324,7 @@
         <v>30</v>
       </c>
       <c r="H24" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1334,7 +1335,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>C0_WF4_biomek-R24</t>
+          <t>C0.1_WF4_biomek-R24</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1360,7 +1361,7 @@
         <v>30</v>
       </c>
       <c r="H25" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1371,7 +1372,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>C0_WA5_manual-R1</t>
+          <t>C0.1_WA5_manual-R1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1397,7 +1398,7 @@
         <v>30</v>
       </c>
       <c r="H26" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1408,7 +1409,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>C0_WB5_manual-R2</t>
+          <t>C0.1_WB5_manual-R2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1434,7 +1435,7 @@
         <v>30</v>
       </c>
       <c r="H27" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1445,7 +1446,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>C0_WC5_manual-R3</t>
+          <t>C0.1_WC5_manual-R3</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1471,7 +1472,7 @@
         <v>30</v>
       </c>
       <c r="H28" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1482,7 +1483,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>C0_WD5_manual-R4</t>
+          <t>C0.1_WD5_manual-R4</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1508,7 +1509,7 @@
         <v>30</v>
       </c>
       <c r="H29" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1519,7 +1520,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>C0_WE5_manual-R5</t>
+          <t>C0.1_WE5_manual-R5</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1545,7 +1546,7 @@
         <v>30</v>
       </c>
       <c r="H30" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1556,7 +1557,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>C0_WF5_manual-R6</t>
+          <t>C0.1_WF5_manual-R6</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1582,7 +1583,7 @@
         <v>30</v>
       </c>
       <c r="H31" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1593,7 +1594,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>C0_WA6_manual-R7</t>
+          <t>C0.1_WA6_manual-R7</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1619,7 +1620,7 @@
         <v>30</v>
       </c>
       <c r="H32" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -1630,7 +1631,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>C0_WB6_manual-R8</t>
+          <t>C0.1_WB6_manual-R8</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1656,7 +1657,7 @@
         <v>30</v>
       </c>
       <c r="H33" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -1667,7 +1668,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>C0_WC6_manual-R9</t>
+          <t>C0.1_WC6_manual-R9</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1693,7 +1694,7 @@
         <v>30</v>
       </c>
       <c r="H34" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -1704,7 +1705,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>C0_WD6_manual-R10</t>
+          <t>C0.1_WD6_manual-R10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1730,7 +1731,7 @@
         <v>30</v>
       </c>
       <c r="H35" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -1741,7 +1742,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>C0_WE6_manual-R11</t>
+          <t>C0.1_WE6_manual-R11</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1767,7 +1768,7 @@
         <v>30</v>
       </c>
       <c r="H36" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -1778,7 +1779,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>C0_WF6_manual-R12</t>
+          <t>C0.1_WF6_manual-R12</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1804,7 +1805,7 @@
         <v>30</v>
       </c>
       <c r="H37" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -1815,7 +1816,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>C0_WA7_manual-R13</t>
+          <t>C0.1_WA7_manual-R13</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1841,7 +1842,7 @@
         <v>30</v>
       </c>
       <c r="H38" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -1852,7 +1853,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>C0_WB7_manual-R14</t>
+          <t>C0.1_WB7_manual-R14</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1878,7 +1879,7 @@
         <v>30</v>
       </c>
       <c r="H39" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -1889,7 +1890,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>C0_WC7_manual-R15</t>
+          <t>C0.1_WC7_manual-R15</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1915,7 +1916,7 @@
         <v>30</v>
       </c>
       <c r="H40" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -1926,7 +1927,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>C0_WD7_manual-R16</t>
+          <t>C0.1_WD7_manual-R16</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1952,7 +1953,7 @@
         <v>30</v>
       </c>
       <c r="H41" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -1963,7 +1964,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>C0_WE7_manual-R17</t>
+          <t>C0.1_WE7_manual-R17</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1989,7 +1990,7 @@
         <v>30</v>
       </c>
       <c r="H42" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2000,7 +2001,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>C0_WF7_manual-R18</t>
+          <t>C0.1_WF7_manual-R18</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2026,7 +2027,7 @@
         <v>30</v>
       </c>
       <c r="H43" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2037,7 +2038,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>C0_WA8_manual-R19</t>
+          <t>C0.1_WA8_manual-R19</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2063,7 +2064,7 @@
         <v>30</v>
       </c>
       <c r="H44" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2074,7 +2075,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>C0_WB8_manual-R20</t>
+          <t>C0.1_WB8_manual-R20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2100,7 +2101,7 @@
         <v>30</v>
       </c>
       <c r="H45" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2111,7 +2112,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>C0_WC8_manual-R21</t>
+          <t>C0.1_WC8_manual-R21</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2137,7 +2138,7 @@
         <v>30</v>
       </c>
       <c r="H46" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2148,7 +2149,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>C0_WD8_manual-R22</t>
+          <t>C0.1_WD8_manual-R22</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2174,7 +2175,7 @@
         <v>30</v>
       </c>
       <c r="H47" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2185,7 +2186,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>C0_WE8_manual-R23</t>
+          <t>C0.1_WE8_manual-R23</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2211,7 +2212,7 @@
         <v>30</v>
       </c>
       <c r="H48" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -2222,7 +2223,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>C0_WF8_manual-R24</t>
+          <t>C0.1_WF8_manual-R24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2248,7 +2249,7 @@
         <v>30</v>
       </c>
       <c r="H49" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -2257,6 +2258,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>